<commit_message>
Update and refactoring 2.0 Datasets
</commit_message>
<xml_diff>
--- a/Dataset/Classifica.xlsx
+++ b/Dataset/Classifica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikym\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniDispense\ICON\ICON_Project\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97321CF5-AAA2-4FF7-B149-A7C129A84198}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3789786D-C4A7-4691-8FA3-C6D3BB8C4CC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4DFF39F0-611F-4906-AD47-C6F4F627D32C}"/>
+    <workbookView xWindow="20370" yWindow="-7305" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{4DFF39F0-611F-4906-AD47-C6F4F627D32C}"/>
   </bookViews>
   <sheets>
     <sheet name="g26" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Romelu Lukaku - 18</t>
   </si>
   <si>
-    <t>Samir HandanoviÄ‡</t>
-  </si>
-  <si>
     <t>Milan</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Cristiano Ronaldo - 20</t>
   </si>
   <si>
-    <t>Wojciech SzczÄ™sny</t>
-  </si>
-  <si>
     <t>Roma</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Jordan Veretout - 10</t>
   </si>
   <si>
-    <t>Pau LÃ³pez</t>
-  </si>
-  <si>
     <t>Atalanta</t>
   </si>
   <si>
@@ -228,9 +219,6 @@
     <t>Roberto Soriano - 8</t>
   </si>
   <si>
-    <t>Åukasz Skorupski</t>
-  </si>
-  <si>
     <t>Genoa</t>
   </si>
   <si>
@@ -261,9 +249,6 @@
     <t>P V P P N</t>
   </si>
   <si>
-    <t>BartÅ‚omiej DrÄ…gowski</t>
-  </si>
-  <si>
     <t>Benevento</t>
   </si>
   <si>
@@ -273,9 +258,6 @@
     <t>Gianluca Caprari - 5</t>
   </si>
   <si>
-    <t>Lorenzo MontipÃ²</t>
-  </si>
-  <si>
     <t>Cagliari</t>
   </si>
   <si>
@@ -463,6 +445,24 @@
   </si>
   <si>
     <t>Dušan Vlahović - 9</t>
+  </si>
+  <si>
+    <t>Samir Handanović</t>
+  </si>
+  <si>
+    <t>Wojciech Szczęsny</t>
+  </si>
+  <si>
+    <t>Pau López</t>
+  </si>
+  <si>
+    <t>Łukasz Skorupski</t>
+  </si>
+  <si>
+    <t>Bartłomiej Drągowski</t>
+  </si>
+  <si>
+    <t>Lorenzo Montipò</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -505,13 +505,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -953,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED23B0F1-C4FB-49D6-B41C-1AD4B0F787DC}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +977,7 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="12" max="12" width="26.140625" customWidth="1"/>
-    <col min="13" max="13" width="24" customWidth="1"/>
+    <col min="13" max="13" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1044,8 +1058,8 @@
       <c r="L2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
-        <v>16</v>
+      <c r="M2" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1053,7 +1067,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>26</v>
@@ -1080,13 +1094,13 @@
         <v>56</v>
       </c>
       <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M3" t="s">
         <v>18</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1094,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -1121,13 +1135,13 @@
         <v>52</v>
       </c>
       <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
+      <c r="M4" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1135,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>26</v>
@@ -1162,13 +1176,13 @@
         <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1176,7 +1190,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>26</v>
@@ -1203,13 +1217,13 @@
         <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1217,7 +1231,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>25</v>
@@ -1244,13 +1258,13 @@
         <v>47</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1258,7 +1272,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>25</v>
@@ -1285,13 +1299,13 @@
         <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1299,7 +1313,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>26</v>
@@ -1326,13 +1340,13 @@
         <v>38</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1340,7 +1354,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -1367,13 +1381,13 @@
         <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1381,7 +1395,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11">
         <v>26</v>
@@ -1408,13 +1422,13 @@
         <v>32</v>
       </c>
       <c r="K11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1422,7 +1436,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12">
         <v>26</v>
@@ -1449,13 +1463,13 @@
         <v>32</v>
       </c>
       <c r="K12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1463,7 +1477,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>26</v>
@@ -1490,13 +1504,13 @@
         <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L13" t="s">
-        <v>57</v>
-      </c>
-      <c r="M13" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1504,7 +1518,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>26</v>
@@ -1531,13 +1545,13 @@
         <v>27</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1545,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15">
         <v>26</v>
@@ -1572,13 +1586,13 @@
         <v>26</v>
       </c>
       <c r="K15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1586,7 +1600,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C16">
         <v>26</v>
@@ -1613,13 +1627,13 @@
         <v>26</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M16" t="s">
-        <v>69</v>
+        <v>130</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1627,7 +1641,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>26</v>
@@ -1654,13 +1668,13 @@
         <v>26</v>
       </c>
       <c r="K17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L17" t="s">
-        <v>72</v>
-      </c>
-      <c r="M17" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1668,7 +1682,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C18">
         <v>26</v>
@@ -1695,13 +1709,13 @@
         <v>22</v>
       </c>
       <c r="K18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1709,7 +1723,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>24</v>
@@ -1736,13 +1750,13 @@
         <v>20</v>
       </c>
       <c r="K19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1750,7 +1764,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>26</v>
@@ -1777,13 +1791,13 @@
         <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="M20" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1791,7 +1805,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C21">
         <v>26</v>
@@ -1818,13 +1832,13 @@
         <v>15</v>
       </c>
       <c r="K21" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L21" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="M21" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1838,7 +1852,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,10 +1948,10 @@
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1945,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>27</v>
@@ -1972,13 +1986,13 @@
         <v>56</v>
       </c>
       <c r="K3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1986,7 +2000,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>26</v>
@@ -2013,13 +2027,13 @@
         <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2027,7 +2041,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>27</v>
@@ -2054,13 +2068,13 @@
         <v>52</v>
       </c>
       <c r="K5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="M5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2068,7 +2082,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>26</v>
@@ -2095,13 +2109,13 @@
         <v>50</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2109,7 +2123,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>27</v>
@@ -2136,13 +2150,13 @@
         <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M7" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2150,7 +2164,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>26</v>
@@ -2177,13 +2191,13 @@
         <v>46</v>
       </c>
       <c r="K8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2191,7 +2205,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>27</v>
@@ -2218,13 +2232,13 @@
         <v>39</v>
       </c>
       <c r="K9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="M9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2232,7 +2246,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>27</v>
@@ -2259,13 +2273,13 @@
         <v>38</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="M10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2273,7 +2287,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11">
         <v>27</v>
@@ -2300,13 +2314,13 @@
         <v>33</v>
       </c>
       <c r="K11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="L11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2314,7 +2328,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>27</v>
@@ -2341,13 +2355,13 @@
         <v>32</v>
       </c>
       <c r="K12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2355,7 +2369,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>27</v>
@@ -2382,13 +2396,13 @@
         <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2396,7 +2410,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>27</v>
@@ -2423,13 +2437,13 @@
         <v>29</v>
       </c>
       <c r="K14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="L14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M14" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2437,7 +2451,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15">
         <v>27</v>
@@ -2464,13 +2478,13 @@
         <v>28</v>
       </c>
       <c r="K15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2478,7 +2492,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16">
         <v>27</v>
@@ -2505,13 +2519,13 @@
         <v>26</v>
       </c>
       <c r="K16" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2519,7 +2533,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>27</v>
@@ -2546,13 +2560,13 @@
         <v>26</v>
       </c>
       <c r="K17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="L17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M17" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2560,7 +2574,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C18">
         <v>26</v>
@@ -2587,13 +2601,13 @@
         <v>23</v>
       </c>
       <c r="K18" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2601,7 +2615,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19">
         <v>27</v>
@@ -2628,13 +2642,13 @@
         <v>22</v>
       </c>
       <c r="K19" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="L19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M19" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2642,7 +2656,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>27</v>
@@ -2669,13 +2683,13 @@
         <v>19</v>
       </c>
       <c r="K20" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="L20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="M20" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2683,7 +2697,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C21">
         <v>27</v>
@@ -2710,13 +2724,13 @@
         <v>15</v>
       </c>
       <c r="K21" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="L21" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="M21" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2732,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6C6C28-59CC-4F00-93C6-7547F99D3B53}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2829,10 +2843,10 @@
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2840,7 +2854,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>28</v>
@@ -2867,13 +2881,13 @@
         <v>59</v>
       </c>
       <c r="K3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="L3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2881,7 +2895,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>28</v>
@@ -2908,13 +2922,13 @@
         <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="L4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2922,7 +2936,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>27</v>
@@ -2949,13 +2963,13 @@
         <v>55</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="L5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M5" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2963,7 +2977,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>27</v>
@@ -2990,13 +3004,13 @@
         <v>53</v>
       </c>
       <c r="K6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3004,7 +3018,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>28</v>
@@ -3031,13 +3045,13 @@
         <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3045,7 +3059,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>27</v>
@@ -3072,13 +3086,13 @@
         <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3086,7 +3100,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>27</v>
@@ -3113,13 +3127,13 @@
         <v>39</v>
       </c>
       <c r="K9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3127,7 +3141,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>28</v>
@@ -3154,13 +3168,13 @@
         <v>38</v>
       </c>
       <c r="K10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="L10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="M10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3168,7 +3182,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11">
         <v>28</v>
@@ -3195,13 +3209,13 @@
         <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="L11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3209,7 +3223,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C12">
         <v>28</v>
@@ -3236,13 +3250,13 @@
         <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="L12" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3250,7 +3264,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>28</v>
@@ -3277,13 +3291,13 @@
         <v>33</v>
       </c>
       <c r="K13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3291,7 +3305,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>28</v>
@@ -3318,13 +3332,13 @@
         <v>31</v>
       </c>
       <c r="K14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -3332,7 +3346,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>28</v>
@@ -3359,13 +3373,13 @@
         <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3373,7 +3387,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16">
         <v>28</v>
@@ -3400,13 +3414,13 @@
         <v>29</v>
       </c>
       <c r="K16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M16" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3414,7 +3428,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>28</v>
@@ -3441,13 +3455,13 @@
         <v>29</v>
       </c>
       <c r="K17" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M17" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -3455,7 +3469,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C18">
         <v>27</v>
@@ -3482,13 +3496,13 @@
         <v>23</v>
       </c>
       <c r="K18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="L18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -3496,7 +3510,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19">
         <v>28</v>
@@ -3523,13 +3537,13 @@
         <v>22</v>
       </c>
       <c r="K19" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="L19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -3537,7 +3551,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>28</v>
@@ -3564,13 +3578,13 @@
         <v>19</v>
       </c>
       <c r="K20" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="M20" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -3578,7 +3592,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C21">
         <v>28</v>
@@ -3605,13 +3619,13 @@
         <v>15</v>
       </c>
       <c r="K21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="M21" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>